<commit_message>
Fix typo in venues
</commit_message>
<xml_diff>
--- a/data/all-venues-3.0.xlsx
+++ b/data/all-venues-3.0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="125">
   <si>
     <t>Paper ID</t>
   </si>
@@ -350,18 +350,9 @@
     <t>Phd Thesis</t>
   </si>
   <si>
-    <t>conference</t>
-  </si>
-  <si>
-    <t>journal</t>
-  </si>
-  <si>
     <t>ICWS</t>
   </si>
   <si>
-    <t>Conference and Workshop Papers</t>
-  </si>
-  <si>
     <t>WISA</t>
   </si>
   <si>
@@ -402,6 +393,12 @@
   </si>
   <si>
     <t>ACSA</t>
+  </si>
+  <si>
+    <t>Conference</t>
+  </si>
+  <si>
+    <t>Journal</t>
   </si>
 </sst>
 </file>
@@ -839,7 +836,7 @@
   <dimension ref="A1:C173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B172" sqref="B172"/>
+      <selection activeCell="A160" sqref="A160:XFD160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +865,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -879,7 +876,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -901,7 +898,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -912,7 +909,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -934,7 +931,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -967,7 +964,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -978,7 +975,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1000,7 +997,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1011,7 +1008,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1022,7 +1019,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1044,7 +1041,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1066,7 +1063,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1077,7 +1074,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1088,7 +1085,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1110,7 +1107,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1121,7 +1118,7 @@
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1132,7 +1129,7 @@
         <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1163,7 +1160,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1185,7 +1182,7 @@
         <v>72</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1196,7 +1193,7 @@
         <v>20</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1216,7 +1213,7 @@
         <v>21</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1227,7 +1224,7 @@
         <v>22</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1238,7 +1235,7 @@
         <v>74</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1249,7 +1246,7 @@
         <v>23</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1260,7 +1257,7 @@
         <v>22</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1271,7 +1268,7 @@
         <v>75</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1282,7 +1279,7 @@
         <v>76</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1293,7 +1290,7 @@
         <v>24</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1304,7 +1301,7 @@
         <v>25</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1315,7 +1312,7 @@
         <v>77</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1326,7 +1323,7 @@
         <v>45</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1337,7 +1334,7 @@
         <v>24</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1348,7 +1345,7 @@
         <v>26</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1359,7 +1356,7 @@
         <v>27</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1370,7 +1367,7 @@
         <v>28</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1381,7 +1378,7 @@
         <v>28</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1392,7 +1389,7 @@
         <v>28</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1403,7 +1400,7 @@
         <v>29</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1414,7 +1411,7 @@
         <v>30</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1425,7 +1422,7 @@
         <v>78</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1436,7 +1433,7 @@
         <v>79</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1447,7 +1444,7 @@
         <v>31</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1458,7 +1455,7 @@
         <v>80</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1480,7 +1477,7 @@
         <v>32</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1513,7 +1510,7 @@
         <v>34</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1524,7 +1521,7 @@
         <v>35</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1535,7 +1532,7 @@
         <v>36</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1546,7 +1543,7 @@
         <v>37</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1557,7 +1554,7 @@
         <v>38</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1568,7 +1565,7 @@
         <v>39</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1579,7 +1576,7 @@
         <v>40</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1590,7 +1587,7 @@
         <v>41</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1601,7 +1598,7 @@
         <v>82</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1612,7 +1609,7 @@
         <v>42</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1645,7 +1642,7 @@
         <v>103</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1667,7 +1664,7 @@
         <v>98</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1678,7 +1675,7 @@
         <v>44</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1689,7 +1686,7 @@
         <v>83</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1731,7 +1728,7 @@
         <v>46</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1742,7 +1739,7 @@
         <v>28</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1773,7 +1770,7 @@
         <v>87</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1793,7 +1790,7 @@
         <v>49</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1804,7 +1801,7 @@
         <v>50</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1815,7 +1812,7 @@
         <v>51</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1826,7 +1823,7 @@
         <v>24</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -1837,7 +1834,7 @@
         <v>36</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1848,7 +1845,7 @@
         <v>88</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1859,7 +1856,7 @@
         <v>15</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1881,7 +1878,7 @@
         <v>89</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1892,7 +1889,7 @@
         <v>89</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -1903,7 +1900,7 @@
         <v>90</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -1925,7 +1922,7 @@
         <v>52</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -1936,7 +1933,7 @@
         <v>53</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -1947,7 +1944,7 @@
         <v>105</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -1958,7 +1955,7 @@
         <v>54</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -1969,7 +1966,7 @@
         <v>91</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -1980,7 +1977,7 @@
         <v>92</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -1991,7 +1988,7 @@
         <v>55</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2013,7 +2010,7 @@
         <v>56</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -2024,7 +2021,7 @@
         <v>99</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -2035,7 +2032,7 @@
         <v>93</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -2046,7 +2043,7 @@
         <v>57</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -2079,7 +2076,7 @@
         <v>94</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -2101,7 +2098,7 @@
         <v>59</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -2112,7 +2109,7 @@
         <v>95</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -2123,7 +2120,7 @@
         <v>60</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -2134,7 +2131,7 @@
         <v>49</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -2167,7 +2164,7 @@
         <v>63</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -2207,7 +2204,7 @@
         <v>64</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -2227,7 +2224,7 @@
         <v>65</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -2267,7 +2264,7 @@
         <v>35</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -2278,7 +2275,7 @@
         <v>49</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -2289,7 +2286,7 @@
         <v>16</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -2300,7 +2297,7 @@
         <v>3</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -2311,7 +2308,7 @@
         <v>97</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -2322,7 +2319,7 @@
         <v>21</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -2333,7 +2330,7 @@
         <v>66</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -2344,7 +2341,7 @@
         <v>100</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -2355,7 +2352,7 @@
         <v>25</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -2366,7 +2363,7 @@
         <v>67</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -2377,7 +2374,7 @@
         <v>68</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -2388,7 +2385,7 @@
         <v>69</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -2399,7 +2396,7 @@
         <v>70</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -2425,10 +2422,10 @@
         <v>558969</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -2439,7 +2436,7 @@
         <v>63</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -2461,7 +2458,7 @@
         <v>15</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -2472,7 +2469,7 @@
         <v>12</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -2489,10 +2486,10 @@
         <v>2117201</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -2500,7 +2497,7 @@
         <v>2352955</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>102</v>
@@ -2553,10 +2550,10 @@
         <v>2353211</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -2564,7 +2561,7 @@
         <v>2353212</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>102</v>
@@ -2578,7 +2575,7 @@
         <v>25</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -2589,7 +2586,7 @@
         <v>49</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -2597,10 +2594,10 @@
         <v>2614324</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -2608,10 +2605,10 @@
         <v>2614539</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -2619,10 +2616,10 @@
         <v>2614833</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -2630,10 +2627,10 @@
         <v>2614909</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -2641,10 +2638,10 @@
         <v>2644180</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -2655,7 +2652,7 @@
         <v>16</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -2663,10 +2660,10 @@
         <v>2644005</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -2677,7 +2674,7 @@
         <v>16</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -2685,7 +2682,7 @@
         <v>2644581</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>102</v>
@@ -2696,10 +2693,10 @@
         <v>3247016</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -2707,10 +2704,10 @@
         <v>3343996</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -2718,10 +2715,10 @@
         <v>3343998</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix typo due to duplicates in venues
</commit_message>
<xml_diff>
--- a/data/all-venues-3.0.xlsx
+++ b/data/all-venues-3.0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="125">
   <si>
     <t>Paper ID</t>
   </si>
@@ -556,8 +556,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:C173" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:C173"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:C171" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C171"/>
   <sortState ref="A2:C166">
     <sortCondition ref="A1:A166"/>
   </sortState>
@@ -833,20 +833,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C173"/>
+  <dimension ref="A1:C171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A160" sqref="A160:XFD160"/>
+      <selection activeCell="A155" sqref="A155:XFD155"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="49.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -857,7 +857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -868,7 +868,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>4</v>
       </c>
@@ -879,7 +879,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>6</v>
       </c>
@@ -890,7 +890,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>10</v>
       </c>
@@ -901,7 +901,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>18</v>
       </c>
@@ -912,7 +912,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>97</v>
       </c>
@@ -923,7 +923,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>98</v>
       </c>
@@ -934,7 +934,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>100</v>
       </c>
@@ -945,7 +945,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>101</v>
       </c>
@@ -956,7 +956,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>102</v>
       </c>
@@ -967,7 +967,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>103</v>
       </c>
@@ -978,7 +978,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>104</v>
       </c>
@@ -989,7 +989,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>106</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>107</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>108</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>109</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>110</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>112</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>113</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>118</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>124</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>128</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>129</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>133</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>139</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>150</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>166</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>178</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>189</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>205</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>245</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>248</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>271</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1894</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>1901</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1906</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1909</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>1913</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>1918</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1926</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1930</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>1934</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1936</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1941</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1942</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1967</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1969</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1971</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1978</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1990</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1992</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>2001</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>2003</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2007</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>2009</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>2014</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2017</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2019</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2021</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2023</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>2028</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>2035</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>2039</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>2040</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>2051</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>2052</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>2053</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>2054</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>2058</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>2076</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>2094</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>2095</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>2096</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>2105</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2106</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>2108</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>2124</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>2127</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>2130</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>2131</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>2142</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>2195</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>2227</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>2252</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>2265</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>2276</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>2277</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>2344</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>2351</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>2392</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>2557</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>2565</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>2566</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>2569</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>2574</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>2586</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>2596</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>2605</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>2673</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>2694</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>2709</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>2720</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>2721</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>2728</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>2731</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>2751</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="2">
         <v>2765</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>2811</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>2816</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>2849</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>2866</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>2904</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>2907</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>2921</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="2">
         <v>2923</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>2932</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>2964</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>2985</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>2996</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>3071</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="2">
         <v>13621</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>13649</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>13682</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>13717</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>14098</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>14136</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="2">
         <v>14145</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>14356</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>14777</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>237068</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>237136</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>265248</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>265374</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="2">
         <v>265471</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>296369</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>296393</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="2">
         <v>296444</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>296464</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>374576</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>471320</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>507542</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>507613</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="2">
         <v>507928</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>507986</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>558969</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>932494</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>1932566</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>1932748</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>1932839</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="5">
         <v>2117185</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>2117201</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>2352955</v>
       </c>
@@ -2503,150 +2503,150 @@
         <v>102</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154">
-        <v>2352968</v>
-      </c>
-      <c r="B154" s="1" t="s">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" s="5">
+        <v>2353028</v>
+      </c>
+      <c r="B154" s="6"/>
+      <c r="C154" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <v>2353203</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C154" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="5">
-        <v>2353028</v>
-      </c>
-      <c r="B155" s="6"/>
-      <c r="C155" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C155" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156">
-        <v>2353177</v>
+        <v>2353211</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157">
-        <v>2353203</v>
+        <v>2353212</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158">
-        <v>2353211</v>
+        <v>2353378</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159">
-        <v>2353212</v>
+        <v>2614321</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160">
-        <v>2353378</v>
+        <v>2614324</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161">
-        <v>2614321</v>
+        <v>2614539</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162">
-        <v>2614324</v>
+        <v>2614833</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C162" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163">
-        <v>2614539</v>
+        <v>2614909</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C163" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164">
-        <v>2614833</v>
+        <v>2644180</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C164" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165">
-        <v>2614909</v>
+        <v>2644233</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166">
-        <v>2644180</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A166" s="5">
+        <v>2644005</v>
+      </c>
+      <c r="B166" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167">
-        <v>2644233</v>
+        <v>2644431</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>16</v>
@@ -2655,69 +2655,47 @@
         <v>123</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="5">
-        <v>2644005</v>
-      </c>
-      <c r="B168" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C168" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169">
-        <v>2644431</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C169" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A168">
+        <v>2644581</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A169" s="5">
+        <v>3247016</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C169" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170">
-        <v>2644581</v>
+        <v>3343996</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="5">
-        <v>3247016</v>
-      </c>
-      <c r="B171" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C171" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172">
-        <v>3343996</v>
-      </c>
-      <c r="B172" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C172" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173">
+      <c r="C170" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171">
         <v>3343998</v>
       </c>
-      <c r="B173" s="1" t="s">
+      <c r="B171" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C173" s="5" t="s">
+      <c r="C171" s="5" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>